<commit_message>
Exclusão de linhas vazias
</commit_message>
<xml_diff>
--- a/Feedback.xlsx
+++ b/Feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barao\Desktop\Insper\CoDes\Projeto_CoDes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F5B9CDB-CE65-49AA-98F0-996882331771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:201_{093C1CFC-1CF3-42AC-9F98-340F3548609F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Descrição do Problema</t>
   </si>
@@ -482,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -557,9 +557,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,19 +792,19 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.453125" style="34" customWidth="1"/>
+    <col min="1" max="1" width="52.453125" style="33" customWidth="1"/>
     <col min="2" max="2" width="34.36328125" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="34"/>
+    <col min="4" max="4" width="32.453125" style="33" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="28"/>
@@ -815,7 +812,7 @@
       <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -827,7 +824,7 @@
       <c r="D2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="33" t="s">
         <v>51</v>
       </c>
     </row>
@@ -844,7 +841,7 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -861,7 +858,7 @@
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -878,7 +875,7 @@
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -895,7 +892,7 @@
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="33" t="s">
         <v>56</v>
       </c>
     </row>
@@ -912,7 +909,7 @@
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -929,7 +926,7 @@
       <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -946,7 +943,7 @@
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -963,7 +960,7 @@
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -980,7 +977,7 @@
       <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -997,7 +994,7 @@
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1014,7 +1011,7 @@
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1031,117 +1028,36 @@
       <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="33" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
-      <c r="B15" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="26">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="30"/>
-      <c r="B16" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="26">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="30"/>
-      <c r="B17" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="26">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
-      <c r="B18" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="26">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
-      <c r="B19" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="26">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20"/>
-      <c r="B20" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="26">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
-      <c r="B21" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="26">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
-      <c r="B22" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="26">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19"/>
-      <c r="B23" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="26">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="27">
-        <f>SUM(C3:C17)</f>
+      <c r="B15" s="29"/>
+      <c r="C15" s="27">
+        <f>SUM(C3:C14)</f>
         <v>33</v>
       </c>
-      <c r="D24" s="3"/>
-    </row>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C3:C23" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C3:C14" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B3:B23" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B14" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>"1. Visibilidade do Status do Sistema,2. Correspondência entre o sistema e o mundo real,3. Controle e Liberdade do Usuário,4. Consistência e Padrões,5. Prevenção de Erros,6. Reconhecimento ao invés de memória,7. Flexibilidade e eficiência de uso,8. Estétic"&amp;"a e design minimalista,9. Recuperação diante de erros,10. Ajuda e Documentação"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Atualização da lista de soluções
</commit_message>
<xml_diff>
--- a/Feedback.xlsx
+++ b/Feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barao\Desktop\Insper\CoDes\Projeto_CoDes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:201_{093C1CFC-1CF3-42AC-9F98-340F3548609F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:201_{26FDFE26-3E20-4276-8CAB-1959430D4EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>Descrição do Problema</t>
   </si>
@@ -207,57 +207,27 @@
   </si>
   <si>
     <t>Adição de h's para indicar horas</t>
+  </si>
+  <si>
+    <t>Mudança dos títulospara TestApp (Working Title)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -290,6 +260,65 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -482,93 +511,96 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -792,256 +824,258 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.453125" style="33" customWidth="1"/>
+    <col min="1" max="1" width="52.453125" style="18" customWidth="1"/>
     <col min="2" max="2" width="34.36328125" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" style="33" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="33"/>
+    <col min="4" max="4" width="32.453125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="28">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:5" ht="76" x14ac:dyDescent="0.35">
+      <c r="A4" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="28">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.35">
+      <c r="A5" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="28">
+        <v>2</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="25" t="s">
+    <row r="6" spans="1:5" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="28">
+        <v>4</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="28">
+        <v>3</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C8" s="28">
+        <v>3</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="63.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="28">
+        <v>4</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="63.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="28">
+        <v>3</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="63.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="28">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="33" t="s">
+      <c r="D11" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="25" t="s">
+    <row r="12" spans="1:5" ht="50" x14ac:dyDescent="0.35">
+      <c r="A12" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="28">
+        <v>2</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="28">
         <v>4</v>
       </c>
-      <c r="C6" s="26">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="26">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="33" t="s">
+      <c r="D13" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="26">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="33" t="s">
+    <row r="14" spans="1:5" ht="50" x14ac:dyDescent="0.35">
+      <c r="A14" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="28">
+        <v>1</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="26">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="26">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="26">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="26">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="26">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="26">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="27">
+      <c r="B15" s="21"/>
+      <c r="C15" s="33">
         <f>SUM(C3:C14)</f>
         <v>33</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1081,184 +1115,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="22"/>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="17"/>
     </row>
     <row r="15" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="15"/>
+      <c r="B19" s="12"/>
     </row>
     <row r="20" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="22"/>
+      <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="14"/>
     </row>
     <row r="22" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="17"/>
+      <c r="B23" s="14"/>
     </row>
     <row r="24" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="12"/>
     </row>
     <row r="26" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="22"/>
+      <c r="B26" s="17"/>
     </row>
     <row r="27" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="14"/>
     </row>
     <row r="28" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="9"/>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="14"/>
     </row>
     <row r="30" spans="1:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>